<commit_message>
fixed LBNRIND, docs and delete check sites
</commit_message>
<xml_diff>
--- a/inst/labs_refer.xlsx
+++ b/inst/labs_refer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\X7-KR\Documents\Rproject\dmtools\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F94F39A-817C-4FD2-ACC6-22CC989D4582}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EFC864A-6B8B-476A-95E2-DB4E81E25C20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,9 +57,6 @@
     <t>LBORRES</t>
   </si>
   <si>
-    <t>LBNDIND</t>
-  </si>
-  <si>
     <t>LBORNRLO</t>
   </si>
   <si>
@@ -82,6 +79,9 @@
   </si>
   <si>
     <t>Aspartate transaminase</t>
+  </si>
+  <si>
+    <t>LBNRIND</t>
   </si>
 </sst>
 </file>
@@ -409,7 +409,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D8" sqref="D8:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -434,13 +434,13 @@
         <v>9</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>11</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -454,13 +454,13 @@
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>2</v>
@@ -480,13 +480,13 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="G3" s="1">
         <v>0</v>
@@ -506,13 +506,13 @@
         <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="G4" s="1">
         <v>0</v>

</xml_diff>